<commit_message>
add fix for tz
</commit_message>
<xml_diff>
--- a/article.xlsx
+++ b/article.xlsx
@@ -1,74 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Work\program\go\src\github.com\RB-PRO\AutoPartsParser\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
-  <si>
-    <t>2Q0953521APIGI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vag </t>
-  </si>
-  <si>
-    <t>57A945307C</t>
-  </si>
-  <si>
-    <t>57A945308C</t>
-  </si>
-  <si>
-    <t>5H0419089EJVDH</t>
-  </si>
-  <si>
-    <t>5H0419089EKVDH</t>
-  </si>
-  <si>
-    <t>5QJ906093</t>
-  </si>
-  <si>
-    <t>57A945207</t>
-  </si>
-  <si>
-    <t>5QF413032B</t>
-  </si>
-  <si>
-    <t>1331259</t>
-  </si>
-  <si>
-    <t>Land Rover</t>
-  </si>
-  <si>
-    <t>LUC100290L</t>
-  </si>
-  <si>
-    <t>LR161110</t>
-  </si>
-  <si>
-    <t>LAND ROVER</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,18 +69,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -437,127 +397,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>1102415</v>
+      </c>
+      <c r="B1" t="str">
+        <v>LAND ROVER</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>LR126119</v>
+      </c>
+      <c r="B2" t="str">
+        <v>LAND ROVER</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B9" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>2Q0953521APIGI</v>
+      </c>
+      <c r="B1" t="str">
+        <v xml:space="preserve">vag </v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>57A945307C</v>
+      </c>
+      <c r="B2" t="str">
+        <v xml:space="preserve">vag </v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>57A945308C</v>
+      </c>
+      <c r="B3" t="str">
+        <v xml:space="preserve">vag </v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>5H0419089EJVDH</v>
+      </c>
+      <c r="B4" t="str">
+        <v xml:space="preserve">vag </v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>5H0419089EKVDH</v>
+      </c>
+      <c r="B5" t="str">
+        <v xml:space="preserve">vag </v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>5QJ906093</v>
+      </c>
+      <c r="B6" t="str">
+        <v xml:space="preserve">vag </v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>57A945207</v>
+      </c>
+      <c r="B7" t="str">
+        <v xml:space="preserve">vag </v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>5QF413032B</v>
+      </c>
+      <c r="B8" t="str">
+        <v xml:space="preserve">vag </v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>1331259</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Land Rover</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>LUC100290L</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Land Rover</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>LR161110</v>
+      </c>
+      <c r="B11" t="str">
+        <v>LAND ROVER</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>LR011343</v>
+      </c>
+      <c r="B12" t="str">
+        <v>LAND ROVER</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError sqref="A1" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add >1 size on parts
</commit_message>
<xml_diff>
--- a/article.xlsx
+++ b/article.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t xml:space="preserve">1102415</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t xml:space="preserve">LR035548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XGB500020</t>
   </si>
   <si>
     <t xml:space="preserve">2Q0953521APIGI</t>
@@ -150,8 +153,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,35 +179,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -226,101 +241,101 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>5</v>
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>5</v>
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>5</v>
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>5</v>
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>5</v>
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>